<commit_message>
Updated autoGenFilter to strictly follow allowed WSG CRUD functions
</commit_message>
<xml_diff>
--- a/iModelBridgeCore/WSClient/ConnectC/Tools/pyApiGen/autoGenFilter.xlsx
+++ b/iModelBridgeCore/WSClient/ConnectC/Tools/pyApiGen/autoGenFilter.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="autoGenFilter" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ECClass Name - must be exactly specified per ECSchema</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>ProjectProperties</t>
+  </si>
+  <si>
+    <t>ProjectTemplate</t>
+  </si>
+  <si>
+    <t>ConnectUser</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -630,7 +639,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -649,6 +658,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -695,473 +707,431 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="68">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+  <dxfs count="62">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6464"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6E0B4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1454,10 +1424,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1466,7 +1436,7 @@
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1484,14 +1454,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
+      <c r="A2" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5" t="b">
         <v>0</v>
@@ -1504,185 +1474,308 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="b">
+      <c r="B3" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="b">
+      <c r="C3" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="b">
+      <c r="D3" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5" t="b">
+        <v>17</v>
+      </c>
+      <c r="B4" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5" t="b">
-        <v>0</v>
+      <c r="C4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5" t="b">
+      <c r="B5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <v>0</v>
+      <c r="D5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="b">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5" t="b">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5" t="b">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="b">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5" t="b">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:E2">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="B7:E14">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:E3">
+    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:E6">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:E4">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:E11">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:E11">
-    <cfRule type="containsText" dxfId="1" priority="-1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="-1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="B2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="B6 B4 B2:E2">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="C2:E2 B3:E11">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="B3:E3 B5 C4:E6 B7:E14">
       <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add ECProperty filter mechanism to pyApiGen tool
</commit_message>
<xml_diff>
--- a/iModelBridgeCore/WSClient/ConnectC/Tools/pyApiGen/autoGenFilter.xlsx
+++ b/iModelBridgeCore/WSClient/ConnectC/Tools/pyApiGen/autoGenFilter.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>ECClass Name - must be exactly specified per ECSchema</t>
   </si>
@@ -73,6 +73,21 @@
   </si>
   <si>
     <t>Project</t>
+  </si>
+  <si>
+    <t>ReadAll</t>
+  </si>
+  <si>
+    <t>NOTE: If all C,R,U,D,ReadAll columns are red (FALSE) for a given row, the corresponding ECClass will be excluded from the API</t>
+  </si>
+  <si>
+    <t>Properties to filter (seperated by commas) - leave empty of no properties should be filtered</t>
+  </si>
+  <si>
+    <t>eBBacked,LinkToAssetType,LinkToIndustry, LinkToIndustryAssets, PWDMInvitationId</t>
+  </si>
+  <si>
+    <t>PWDMInvitationId</t>
   </si>
 </sst>
 </file>
@@ -221,7 +236,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,8 +428,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -594,6 +615,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -639,20 +718,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -660,6 +727,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -707,91 +805,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="62">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6E0B4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6464"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <fill>
         <patternFill>
@@ -1424,358 +1438,556 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.44140625" customWidth="1"/>
+    <col min="1" max="1" width="57.21875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="76.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="B2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="b">
+      <c r="B3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="b">
+      <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="6" t="b">
+      <c r="B4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="b">
+      <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="b">
+      <c r="D4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="b">
+      <c r="E4" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="b">
+      <c r="B5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="b">
+      <c r="D5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="b">
+      <c r="B6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C6" s="6" t="b">
+      <c r="C6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6" t="b">
+      <c r="B7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6" t="b">
-        <v>0</v>
+      <c r="D7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="B8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="B9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="B10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="B11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="B12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="B13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6" t="b">
-        <v>0</v>
-      </c>
+      <c r="B14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:7" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H1:S1"/>
+    <mergeCell ref="A28:F28"/>
+  </mergeCells>
   <conditionalFormatting sqref="B7:E14">
-    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="49" priority="55" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="48" priority="56" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:E3">
-    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="20" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="45" priority="49" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="50" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:E6">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:E4">
+    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="42" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",D5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G2">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:G8">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",D2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F8)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:G9">
     <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:E6">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B6)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",E5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",E5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",D5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",D5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:G10">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:G11">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:G12">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13:G13">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:G14">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:G7">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:G6">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:G5">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:G4">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:G3">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="B6 B4 B2:E2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Please enter TRUE or FALSE" error="Only &quot;TRUE&quot;, or &quot;FALSE&quot; are allowed values. Please enter a valid value." sqref="B6 B4 F8:F14 B2:F2">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="B3:E3 B5 C4:E6 B7:E14">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Enter a valid CRUD function" error="Only &quot;Create&quot;, &quot;Read&quot;, &quot;Update&quot;, or &quot;Delete&quot; are allowed values. Please enter a valid value." sqref="F4:F7 B5 C4:E6 B7:E14 B3:F3">
       <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>